<commit_message>
Initial Draft for Submission
</commit_message>
<xml_diff>
--- a/P01/P01_Documentation.xlsx
+++ b/P01/P01_Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naseef\Documents\MPLABXProjects\Projects\P01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BAE7EC5-2539-439F-8444-F1C9C0762F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA02726-EE30-4F04-AFDA-03D7991AAF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{5A5CEE6C-12C7-448E-A7AD-903EE24D137B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>SL NO.</t>
   </si>
@@ -124,18 +124,12 @@
     <t>Printed "Resetting…" in LCD and resumed from test case 2</t>
   </si>
   <si>
-    <t>Test Case</t>
-  </si>
-  <si>
     <t>Switch of device if push button presses exceeds 10 counts</t>
   </si>
   <si>
     <t xml:space="preserve">Printing low battery, reminder to recharge and switching off messages in screen and go blank screen </t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>CORNER CASE</t>
   </si>
   <si>
@@ -152,6 +146,21 @@
   </si>
   <si>
     <t>Printed "!!!CLOUDY ENVIRONMENT!!! In first line and "CAN'T FETCH DATA" in second line. Then resetting message in last two lines</t>
+  </si>
+  <si>
+    <t>Test Case 6</t>
+  </si>
+  <si>
+    <t>Test Case 7</t>
+  </si>
+  <si>
+    <t>Show Reset counts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when push button presses, count the number of presses </t>
+  </si>
+  <si>
+    <t>No. Presses displayed on a 7-Segment Display</t>
   </si>
 </sst>
 </file>
@@ -168,15 +177,14 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -203,18 +211,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5063C89-A2E3-44B1-80C1-768AFD562496}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,12 +551,12 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="46.140625" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" customWidth="1"/>
-    <col min="5" max="5" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -557,7 +566,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -577,172 +586,204 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="84" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
+      <c r="F13" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>